<commit_message>
Dynamic Report Contents setup HP
</commit_message>
<xml_diff>
--- a/BaseFiles/Template_4.xlsx
+++ b/BaseFiles/Template_4.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hostbv833-my.sharepoint.com/personal/v_kroeze_bright-renewables_com/Documents/v.kroeze/UITZOEKEN/Monthly reporting tool/BaseFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hostbv833-my.sharepoint.com/personal/g_vandoorn_bright-renewables_com/Documents/Documenten/Python Scripts/BURP/BaseFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{48B7B004-DE07-47AA-894B-01E1C6DC16B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4333EF52-BFBC-4442-B100-DF9BC1B9F1E1}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{48B7B004-DE07-47AA-894B-01E1C6DC16B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{570FDE14-B7E4-4F4E-9C29-0F3CF94098C4}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3480E52E-072E-4D59-A71C-9A9899EEDC18}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3480E52E-072E-4D59-A71C-9A9899EEDC18}"/>
   </bookViews>
   <sheets>
     <sheet name="Rapportage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="500"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -325,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -363,10 +363,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,9 +391,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>361314</xdr:colOff>
+      <xdr:colOff>365124</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>137159</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -435,7 +434,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -736,8 +735,8 @@
   </sheetPr>
   <dimension ref="B3:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1060,7 +1059,7 @@
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="27" t="s">
+      <c r="G28" s="15" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="23"/>

</xml_diff>